<commit_message>
bugfix: kill card and move to grave before play card to slot causing remove null from card slot; constrain card playability to slots by color
</commit_message>
<xml_diff>
--- a/Server/assets/data.xlsx
+++ b/Server/assets/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Card" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Decks" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Card!$A$1:$O$1000</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Card!$A$1:$P$1000</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="511">
   <si>
     <t>Cost</t>
   </si>
@@ -1545,10 +1545,19 @@
     <t>对目标生物或者玩家造成4点伤害，你所操控的每一个红色生物对你的目标造成1点伤害|n&lt;b&gt;施法结束时：&lt;/b&gt;回到手牌</t>
   </si>
   <si>
-    <t>置于蓝色卡槽，卡槽效果额外降低1点敌方力量判定</t>
-  </si>
-  <si>
     <t>Marsh Barrier</t>
+  </si>
+  <si>
+    <t>置于蓝色卡槽，在战斗时降低1点敌方力量判定</t>
+  </si>
+  <si>
+    <t>allowslot</t>
+  </si>
+  <si>
+    <t>all,blue,red,white,green</t>
+  </si>
+  <si>
+    <t>all,blue</t>
   </si>
 </sst>
 </file>
@@ -2052,10 +2061,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1" filterMode="1"/>
-  <dimension ref="A1:O1000"/>
+  <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,19 +2075,20 @@
     <col min="4" max="4" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="88.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="70.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="7" width="7.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="88.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="70.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>332</v>
       </c>
@@ -2098,34 +2108,37 @@
         <v>336</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="11" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1000124</v>
       </c>
@@ -2145,28 +2158,31 @@
         <v>415</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>0</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>1</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1000125</v>
       </c>
@@ -2183,22 +2199,25 @@
         <v>415</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>0</v>
       </c>
-      <c r="J3" s="2">
-        <v>2</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="2">
+        <v>2</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1000126</v>
       </c>
@@ -2218,22 +2237,25 @@
         <v>415</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>0</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1000002</v>
       </c>
@@ -2253,23 +2275,26 @@
         <v>415</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I5" s="4">
-        <v>1</v>
       </c>
       <c r="J5" s="4">
         <v>1</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>1000023</v>
       </c>
@@ -2277,7 +2302,7 @@
         <v>414</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>2</v>
@@ -2289,23 +2314,26 @@
         <v>415</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="4">
         <v>1</v>
       </c>
-      <c r="J6" s="4">
-        <v>2</v>
-      </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="4">
+        <v>2</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>463</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="M6" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>1000028</v>
       </c>
@@ -2325,21 +2353,24 @@
         <v>415</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="4">
         <v>1</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="M7" s="12" t="s">
         <v>460</v>
       </c>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>1000119</v>
       </c>
@@ -2359,22 +2390,25 @@
         <v>415</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
       </c>
       <c r="J8" s="2">
         <v>1</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>1000118</v>
       </c>
@@ -2394,19 +2428,22 @@
         <v>415</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I9" s="2">
-        <v>1</v>
       </c>
       <c r="J9" s="2">
         <v>1</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>1000123</v>
       </c>
@@ -2426,19 +2463,22 @@
         <v>415</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>1</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>1000046</v>
       </c>
@@ -2458,21 +2498,24 @@
         <v>415</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="4">
         <v>1</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="M11" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>1000004</v>
       </c>
@@ -2491,25 +2534,28 @@
       <c r="F12" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9">
-        <v>2</v>
-      </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9" t="s">
+      <c r="I12" s="8"/>
+      <c r="J12" s="9">
+        <v>2</v>
+      </c>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="M12" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="10"/>
-    </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="8"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1000005</v>
       </c>
@@ -2529,23 +2575,26 @@
         <v>415</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I13" s="4">
-        <v>2</v>
-      </c>
       <c r="J13" s="4">
         <v>2</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="4">
+        <v>2</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="L13" s="12"/>
-      <c r="O13" s="3" t="s">
+      <c r="M13" s="12"/>
+      <c r="P13" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>1000013</v>
       </c>
@@ -2565,26 +2614,29 @@
         <v>415</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="4">
-        <v>2</v>
-      </c>
+      <c r="I14" s="2"/>
       <c r="J14" s="4">
+        <v>2</v>
+      </c>
+      <c r="K14" s="4">
         <v>1</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="L14" s="12" t="s">
+      <c r="M14" s="12" t="s">
         <v>359</v>
       </c>
-      <c r="M14" s="2"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O14" s="2"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>1000011</v>
       </c>
@@ -2604,23 +2656,26 @@
         <v>415</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I15" s="4">
-        <v>2</v>
-      </c>
       <c r="J15" s="4">
         <v>2</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="4">
+        <v>2</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="M15" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>1000030</v>
       </c>
@@ -2640,21 +2695,24 @@
         <v>415</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I16" s="4">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3" t="s">
+      <c r="J16" s="4">
+        <v>2</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="L16" s="12" t="s">
-        <v>506</v>
-      </c>
-      <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="12" t="s">
+        <v>507</v>
+      </c>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>1000043</v>
       </c>
@@ -2674,21 +2732,24 @@
         <v>415</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I17" s="4">
-        <v>2</v>
-      </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4" t="s">
+      <c r="J17" s="4">
+        <v>2</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="M17" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>1000029</v>
       </c>
@@ -2708,23 +2769,26 @@
         <v>415</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I18" s="4">
-        <v>2</v>
-      </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3" t="s">
+      <c r="J18" s="4">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L18" s="12" t="s">
+      <c r="M18" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="O18" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>1000010</v>
       </c>
@@ -2744,23 +2808,26 @@
         <v>415</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I19" s="4">
-        <v>3</v>
       </c>
       <c r="J19" s="4">
         <v>3</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="4">
+        <v>3</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="L19" s="12" t="s">
+      <c r="M19" s="12" t="s">
         <v>483</v>
       </c>
-      <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>1000016</v>
       </c>
@@ -2780,23 +2847,26 @@
         <v>415</v>
       </c>
       <c r="G20" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I20" s="4">
+      <c r="J20" s="4">
         <v>3</v>
       </c>
-      <c r="J20" s="4">
-        <v>2</v>
-      </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="4">
+        <v>2</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="L20" s="12" t="s">
+      <c r="M20" s="12" t="s">
         <v>288</v>
       </c>
-      <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1000017</v>
       </c>
@@ -2816,23 +2886,26 @@
         <v>415</v>
       </c>
       <c r="G21" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I21" s="4">
-        <v>3</v>
       </c>
       <c r="J21" s="4">
         <v>3</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="4">
+        <v>3</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="M21" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="3"/>
+    </row>
+    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>1000012</v>
       </c>
@@ -2852,21 +2925,24 @@
         <v>415</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I22" s="4">
+      <c r="J22" s="4">
         <v>3</v>
       </c>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="4"/>
+      <c r="L22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L22" s="12" t="s">
+      <c r="M22" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>1000040</v>
       </c>
@@ -2886,21 +2962,24 @@
         <v>415</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I23" s="4">
+      <c r="J23" s="4">
         <v>3</v>
       </c>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="4"/>
+      <c r="L23" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L23" s="12" t="s">
+      <c r="M23" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="3"/>
+    </row>
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>1000003</v>
       </c>
@@ -2919,25 +2998,28 @@
       <c r="F24" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="H24" s="7"/>
-      <c r="I24" s="9">
+      <c r="I24" s="7"/>
+      <c r="J24" s="9">
         <v>3</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9" t="s">
+      <c r="K24" s="9"/>
+      <c r="L24" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="M24" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="M24" s="7"/>
       <c r="N24" s="7"/>
-      <c r="O24" s="10"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O24" s="7"/>
+      <c r="P24" s="10"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>1000048</v>
       </c>
@@ -2957,21 +3039,24 @@
         <v>415</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I25" s="4">
+      <c r="J25" s="4">
         <v>3</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="4"/>
+      <c r="L25" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="M25" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>1000001</v>
       </c>
@@ -2991,23 +3076,26 @@
         <v>415</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I26" s="4">
+      <c r="J26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>0</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="L26" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="L26" s="12" t="s">
+      <c r="M26" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>1000020</v>
       </c>
@@ -3027,23 +3115,26 @@
         <v>415</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I27" s="4">
+      <c r="J27" s="4">
         <v>4</v>
       </c>
-      <c r="J27" s="4">
+      <c r="K27" s="4">
         <v>3</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="L27" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="L27" s="12" t="s">
+      <c r="M27" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>1000044</v>
       </c>
@@ -3063,23 +3154,26 @@
         <v>415</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I28" s="4">
+      <c r="J28" s="4">
         <v>4</v>
       </c>
-      <c r="J28" s="4">
+      <c r="K28" s="4">
         <v>3</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="L28" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="L28" s="12" t="s">
+      <c r="M28" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>1000039</v>
       </c>
@@ -3099,21 +3193,24 @@
         <v>415</v>
       </c>
       <c r="G29" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I29" s="4">
+      <c r="J29" s="4">
         <v>4</v>
       </c>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="4"/>
+      <c r="L29" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L29" s="12" t="s">
+      <c r="M29" s="12" t="s">
         <v>291</v>
       </c>
-      <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>1000042</v>
       </c>
@@ -3133,24 +3230,27 @@
         <v>415</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="4">
+      <c r="I30" s="2"/>
+      <c r="J30" s="4">
         <v>4</v>
       </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="4"/>
+      <c r="L30" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L30" s="12" t="s">
+      <c r="M30" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="M30" s="2"/>
       <c r="N30" s="2"/>
-      <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="O30" s="2"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>1000127</v>
       </c>
@@ -3170,19 +3270,22 @@
         <v>415</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>4</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="M31" s="2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>1000045</v>
       </c>
@@ -3202,21 +3305,24 @@
         <v>415</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I32" s="4">
+      <c r="J32" s="4">
         <v>5</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="4"/>
+      <c r="L32" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L32" s="12" t="s">
+      <c r="M32" s="12" t="s">
         <v>475</v>
       </c>
-      <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>1000021</v>
       </c>
@@ -3236,23 +3342,26 @@
         <v>415</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I33" s="4">
+      <c r="J33" s="4">
         <v>5</v>
       </c>
-      <c r="J33" s="4">
+      <c r="K33" s="4">
         <v>3</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="L33" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="L33" s="12" t="s">
+      <c r="M33" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1000024</v>
       </c>
@@ -3272,23 +3381,26 @@
         <v>415</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I34" s="4">
+      <c r="J34" s="4">
         <v>5</v>
       </c>
-      <c r="J34" s="4">
+      <c r="K34" s="4">
         <v>4</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="L34" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="L34" s="12" t="s">
+      <c r="M34" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>1000047</v>
       </c>
@@ -3308,23 +3420,26 @@
         <v>415</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I35" s="4">
+      <c r="J35" s="4">
         <v>5</v>
       </c>
-      <c r="J35" s="4">
+      <c r="K35" s="4">
         <v>3</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="L35" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="L35" s="12" t="s">
+      <c r="M35" s="12" t="s">
         <v>478</v>
       </c>
-      <c r="O35" s="3"/>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1000019</v>
       </c>
@@ -3344,23 +3459,26 @@
         <v>415</v>
       </c>
       <c r="G36" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I36" s="4">
-        <v>6</v>
       </c>
       <c r="J36" s="4">
         <v>6</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="K36" s="4">
+        <v>6</v>
+      </c>
+      <c r="L36" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="L36" s="12" t="s">
+      <c r="M36" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="O36" s="3"/>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>1000027</v>
       </c>
@@ -3380,23 +3498,26 @@
         <v>415</v>
       </c>
       <c r="G37" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I37" s="4">
-        <v>6</v>
       </c>
       <c r="J37" s="4">
         <v>6</v>
       </c>
-      <c r="K37" s="4" t="s">
+      <c r="K37" s="4">
+        <v>6</v>
+      </c>
+      <c r="L37" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="L37" s="12" t="s">
+      <c r="M37" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="O37" s="3"/>
-    </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P37" s="3"/>
+    </row>
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>1000120</v>
       </c>
@@ -3416,22 +3537,25 @@
         <v>415</v>
       </c>
       <c r="G38" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H38" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>7</v>
       </c>
-      <c r="J38" s="2">
+      <c r="K38" s="2">
         <v>9</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="L38" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="M38" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>1000121</v>
       </c>
@@ -3451,22 +3575,25 @@
         <v>415</v>
       </c>
       <c r="G39" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H39" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I39" s="2">
-        <v>7</v>
       </c>
       <c r="J39" s="2">
         <v>7</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="K39" s="2">
+        <v>7</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>1000122</v>
       </c>
@@ -3486,22 +3613,25 @@
         <v>415</v>
       </c>
       <c r="G40" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="2">
         <v>8</v>
       </c>
-      <c r="J40" s="2">
+      <c r="K40" s="2">
         <v>4</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="L40" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="M40" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>1000132</v>
       </c>
@@ -3521,22 +3651,25 @@
         <v>416</v>
       </c>
       <c r="G41" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H41" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="I41" s="2">
+      <c r="J41" s="2">
         <v>0</v>
       </c>
-      <c r="J41" s="2">
+      <c r="K41" s="2">
         <v>3</v>
       </c>
-      <c r="K41" s="2" t="s">
+      <c r="L41" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>1000136</v>
       </c>
@@ -3556,22 +3689,25 @@
         <v>416</v>
       </c>
       <c r="G42" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>0</v>
       </c>
-      <c r="J42" s="2">
+      <c r="K42" s="2">
         <v>1</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>1000006</v>
       </c>
@@ -3591,23 +3727,26 @@
         <v>416</v>
       </c>
       <c r="G43" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I43" s="4">
-        <v>1</v>
       </c>
       <c r="J43" s="4">
         <v>1</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K43" s="4">
+        <v>1</v>
+      </c>
+      <c r="L43" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="L43" s="12" t="s">
+      <c r="M43" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="O43" s="3"/>
-    </row>
-    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P43" s="3"/>
+    </row>
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>1000014</v>
       </c>
@@ -3627,23 +3766,26 @@
         <v>416</v>
       </c>
       <c r="G44" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I44" s="4">
-        <v>1</v>
       </c>
       <c r="J44" s="4">
         <v>1</v>
       </c>
-      <c r="K44" s="4" t="s">
+      <c r="K44" s="4">
+        <v>1</v>
+      </c>
+      <c r="L44" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="L44" s="12" t="s">
+      <c r="M44" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="O44" s="4"/>
-    </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P44" s="4"/>
+    </row>
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>1000053</v>
       </c>
@@ -3663,22 +3805,25 @@
         <v>416</v>
       </c>
       <c r="G45" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H45" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I45" s="2">
+      <c r="J45" s="2">
         <v>1</v>
       </c>
-      <c r="J45" s="2">
+      <c r="K45" s="2">
         <v>0</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L45" s="2" t="s">
+      <c r="M45" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>1000128</v>
       </c>
@@ -3698,19 +3843,22 @@
         <v>416</v>
       </c>
       <c r="G46" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H46" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I46" s="2">
+      <c r="J46" s="2">
         <v>1</v>
       </c>
-      <c r="J46" s="2">
-        <v>2</v>
-      </c>
-      <c r="K46" s="2" t="s">
+      <c r="K46" s="2">
+        <v>2</v>
+      </c>
+      <c r="L46" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>1000129</v>
       </c>
@@ -3730,22 +3878,25 @@
         <v>416</v>
       </c>
       <c r="G47" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H47" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I47" s="2">
-        <v>1</v>
       </c>
       <c r="J47" s="2">
         <v>1</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="K47" s="2">
+        <v>1</v>
+      </c>
+      <c r="L47" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L47" s="2" t="s">
+      <c r="M47" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>1000007</v>
       </c>
@@ -3765,23 +3916,26 @@
         <v>416</v>
       </c>
       <c r="G48" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="I48" s="4">
-        <v>1</v>
       </c>
       <c r="J48" s="4">
         <v>1</v>
       </c>
-      <c r="K48" s="4" t="s">
+      <c r="K48" s="4">
+        <v>1</v>
+      </c>
+      <c r="L48" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L48" s="12" t="s">
+      <c r="M48" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="O48" s="3"/>
-    </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P48" s="3"/>
+    </row>
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>1000055</v>
       </c>
@@ -3800,25 +3954,28 @@
       <c r="F49" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="G49" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H49" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6">
+      <c r="I49" s="6"/>
+      <c r="J49" s="6">
         <v>1</v>
       </c>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6" t="s">
+      <c r="K49" s="6"/>
+      <c r="L49" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="L49" s="6" t="s">
+      <c r="M49" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="M49" s="6"/>
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
-    </row>
-    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P49" s="6"/>
+    </row>
+    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>1000056</v>
       </c>
@@ -3838,19 +3995,22 @@
         <v>416</v>
       </c>
       <c r="G50" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I50" s="2">
+      <c r="J50" s="2">
         <v>1</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L50" s="2" t="s">
+      <c r="M50" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>1000052</v>
       </c>
@@ -3870,22 +4030,25 @@
         <v>416</v>
       </c>
       <c r="G51" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="I51" s="2">
-        <v>2</v>
-      </c>
       <c r="J51" s="2">
         <v>2</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="K51" s="2">
+        <v>2</v>
+      </c>
+      <c r="L51" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>1000058</v>
       </c>
@@ -3905,25 +4068,28 @@
         <v>416</v>
       </c>
       <c r="G52" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H52" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="I52" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="I52" s="2">
-        <v>2</v>
-      </c>
       <c r="J52" s="2">
+        <v>2</v>
+      </c>
+      <c r="K52" s="2">
         <v>1</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="L52" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L52" s="2" t="s">
+      <c r="M52" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>1000060</v>
       </c>
@@ -3943,22 +4109,25 @@
         <v>416</v>
       </c>
       <c r="G53" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H53" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I53" s="2">
-        <v>2</v>
-      </c>
       <c r="J53" s="2">
+        <v>2</v>
+      </c>
+      <c r="K53" s="2">
         <v>1</v>
       </c>
-      <c r="K53" s="2" t="s">
+      <c r="L53" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L53" s="2" t="s">
+      <c r="M53" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>1000065</v>
       </c>
@@ -3978,22 +4147,25 @@
         <v>416</v>
       </c>
       <c r="G54" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I54" s="2">
-        <v>2</v>
-      </c>
       <c r="J54" s="2">
+        <v>2</v>
+      </c>
+      <c r="K54" s="2">
         <v>1</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="L54" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L54" s="2" t="s">
+      <c r="M54" s="2" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>1000031</v>
       </c>
@@ -4013,21 +4185,24 @@
         <v>416</v>
       </c>
       <c r="G55" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H55" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I55" s="4">
-        <v>2</v>
-      </c>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3" t="s">
+      <c r="J55" s="4">
+        <v>2</v>
+      </c>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="L55" s="12" t="s">
+      <c r="M55" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="O55" s="3"/>
-    </row>
-    <row r="56" spans="1:15" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P55" s="3"/>
+    </row>
+    <row r="56" spans="1:16" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>1000062</v>
       </c>
@@ -4047,24 +4222,27 @@
         <v>416</v>
       </c>
       <c r="G56" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2">
-        <v>2</v>
-      </c>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2" t="s">
+      <c r="I56" s="2"/>
+      <c r="J56" s="2">
+        <v>2</v>
+      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L56" s="2" t="s">
+      <c r="M56" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="M56" s="2"/>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
-    </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P56" s="2"/>
+    </row>
+    <row r="57" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>1000018</v>
       </c>
@@ -4084,23 +4262,26 @@
         <v>416</v>
       </c>
       <c r="G57" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I57" s="4">
+      <c r="J57" s="4">
         <v>3</v>
       </c>
-      <c r="J57" s="4">
-        <v>2</v>
-      </c>
-      <c r="K57" s="4" t="s">
+      <c r="K57" s="4">
+        <v>2</v>
+      </c>
+      <c r="L57" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="L57" s="12" t="s">
+      <c r="M57" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="O57" s="3"/>
-    </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P57" s="3"/>
+    </row>
+    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>1000059</v>
       </c>
@@ -4120,22 +4301,25 @@
         <v>416</v>
       </c>
       <c r="G58" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H58" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="I58" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="I58" s="2">
+      <c r="J58" s="2">
         <v>3</v>
       </c>
-      <c r="J58" s="2">
+      <c r="K58" s="2">
         <v>4</v>
       </c>
-      <c r="K58" s="2" t="s">
+      <c r="L58" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>1000067</v>
       </c>
@@ -4155,25 +4339,28 @@
         <v>416</v>
       </c>
       <c r="G59" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H59" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="I59" s="2">
+      <c r="J59" s="2">
         <v>3</v>
       </c>
-      <c r="J59" s="2">
-        <v>2</v>
-      </c>
-      <c r="K59" s="2" t="s">
+      <c r="K59" s="2">
+        <v>2</v>
+      </c>
+      <c r="L59" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L59" s="2" t="s">
+      <c r="M59" s="2" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>1000063</v>
       </c>
@@ -4193,19 +4380,22 @@
         <v>416</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I60" s="2">
+      <c r="J60" s="2">
         <v>3</v>
       </c>
-      <c r="K60" s="2" t="s">
+      <c r="L60" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L60" s="2" t="s">
+      <c r="M60" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>1000054</v>
       </c>
@@ -4225,19 +4415,22 @@
         <v>416</v>
       </c>
       <c r="G61" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I61" s="2">
+      <c r="J61" s="2">
         <v>3</v>
       </c>
-      <c r="K61" s="2" t="s">
+      <c r="L61" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L61" s="2" t="s">
+      <c r="M61" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>1000064</v>
       </c>
@@ -4257,19 +4450,22 @@
         <v>416</v>
       </c>
       <c r="G62" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I62" s="2">
+      <c r="J62" s="2">
         <v>3</v>
       </c>
-      <c r="K62" s="2" t="s">
+      <c r="L62" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L62" s="2" t="s">
+      <c r="M62" s="2" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>1000068</v>
       </c>
@@ -4289,19 +4485,22 @@
         <v>416</v>
       </c>
       <c r="G63" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I63" s="2">
+      <c r="J63" s="2">
         <v>3</v>
       </c>
-      <c r="K63" s="2" t="s">
+      <c r="L63" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L63" s="2" t="s">
+      <c r="M63" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>1000061</v>
       </c>
@@ -4321,22 +4520,25 @@
         <v>416</v>
       </c>
       <c r="G64" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H64" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I64" s="2">
+      <c r="J64" s="2">
         <v>4</v>
       </c>
-      <c r="J64" s="2">
+      <c r="K64" s="2">
         <v>3</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="L64" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L64" s="2" t="s">
+      <c r="M64" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>1000066</v>
       </c>
@@ -4356,22 +4558,25 @@
         <v>416</v>
       </c>
       <c r="G65" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H65" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I65" s="2">
+      <c r="J65" s="2">
         <v>4</v>
       </c>
-      <c r="J65" s="2">
+      <c r="K65" s="2">
         <v>3</v>
       </c>
-      <c r="K65" s="2" t="s">
+      <c r="L65" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L65" s="2" t="s">
+      <c r="M65" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>1000070</v>
       </c>
@@ -4391,22 +4596,25 @@
         <v>416</v>
       </c>
       <c r="G66" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H66" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I66" s="2">
-        <v>4</v>
       </c>
       <c r="J66" s="2">
         <v>4</v>
       </c>
-      <c r="K66" s="2" t="s">
+      <c r="K66" s="2">
+        <v>4</v>
+      </c>
+      <c r="L66" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L66" s="2" t="s">
+      <c r="M66" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>1000071</v>
       </c>
@@ -4426,22 +4634,25 @@
         <v>416</v>
       </c>
       <c r="G67" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H67" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I67" s="2">
+      <c r="J67" s="2">
         <v>4</v>
       </c>
-      <c r="J67" s="2">
-        <v>2</v>
-      </c>
-      <c r="K67" s="2" t="s">
+      <c r="K67" s="2">
+        <v>2</v>
+      </c>
+      <c r="L67" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L67" s="2" t="s">
+      <c r="M67" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>1000057</v>
       </c>
@@ -4461,19 +4672,22 @@
         <v>416</v>
       </c>
       <c r="G68" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H68" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I68" s="2">
+      <c r="J68" s="2">
         <v>4</v>
       </c>
-      <c r="K68" s="2" t="s">
+      <c r="L68" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L68" s="2" t="s">
+      <c r="M68" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7">
         <v>1000073</v>
       </c>
@@ -4493,19 +4707,22 @@
         <v>416</v>
       </c>
       <c r="G69" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H69" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I69" s="2">
+      <c r="J69" s="2">
         <v>4</v>
       </c>
-      <c r="K69" s="2" t="s">
+      <c r="L69" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L69" s="2" t="s">
+      <c r="M69" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>1000025</v>
       </c>
@@ -4525,23 +4742,26 @@
         <v>416</v>
       </c>
       <c r="G70" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H70" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I70" s="4">
-        <v>5</v>
       </c>
       <c r="J70" s="4">
         <v>5</v>
       </c>
-      <c r="K70" s="4" t="s">
+      <c r="K70" s="4">
+        <v>5</v>
+      </c>
+      <c r="L70" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="L70" s="2" t="s">
+      <c r="M70" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="O70" s="3"/>
-    </row>
-    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P70" s="3"/>
+    </row>
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7">
         <v>1000133</v>
       </c>
@@ -4561,22 +4781,25 @@
         <v>416</v>
       </c>
       <c r="G71" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H71" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I71" s="2">
+      <c r="J71" s="2">
         <v>5</v>
       </c>
-      <c r="J71" s="2">
+      <c r="K71" s="2">
         <v>4</v>
       </c>
-      <c r="K71" s="2" t="s">
+      <c r="L71" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L71" s="2" t="s">
+      <c r="M71" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7">
         <v>1000134</v>
       </c>
@@ -4596,22 +4819,25 @@
         <v>416</v>
       </c>
       <c r="G72" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H72" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I72" s="2">
+      <c r="J72" s="2">
         <v>5</v>
       </c>
-      <c r="J72" s="2">
+      <c r="K72" s="2">
         <v>4</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="L72" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L72" s="2" t="s">
+      <c r="M72" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7">
         <v>1000135</v>
       </c>
@@ -4631,19 +4857,22 @@
         <v>416</v>
       </c>
       <c r="G73" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H73" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I73" s="2">
+      <c r="J73" s="2">
         <v>5</v>
       </c>
-      <c r="K73" s="2" t="s">
+      <c r="L73" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L73" s="2" t="s">
+      <c r="M73" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7">
         <v>1000069</v>
       </c>
@@ -4663,22 +4892,25 @@
         <v>416</v>
       </c>
       <c r="G74" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H74" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I74" s="2">
-        <v>6</v>
       </c>
       <c r="J74" s="2">
         <v>6</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="K74" s="2">
+        <v>6</v>
+      </c>
+      <c r="L74" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="L74" s="2" t="s">
+      <c r="M74" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7">
         <v>1000074</v>
       </c>
@@ -4698,22 +4930,25 @@
         <v>416</v>
       </c>
       <c r="G75" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H75" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I75" s="2">
+      <c r="J75" s="2">
         <v>6</v>
       </c>
-      <c r="J75" s="2">
+      <c r="K75" s="2">
         <v>5</v>
       </c>
-      <c r="K75" s="2" t="s">
+      <c r="L75" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L75" s="2" t="s">
+      <c r="M75" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7">
         <v>1000072</v>
       </c>
@@ -4733,25 +4968,28 @@
         <v>416</v>
       </c>
       <c r="G76" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H76" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="I76" s="2">
+      <c r="J76" s="2">
         <v>7</v>
       </c>
-      <c r="J76" s="2">
+      <c r="K76" s="2">
         <v>8</v>
       </c>
-      <c r="K76" s="2" t="s">
+      <c r="L76" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L76" s="2" t="s">
+      <c r="M76" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
         <v>1000131</v>
       </c>
@@ -4771,25 +5009,28 @@
         <v>416</v>
       </c>
       <c r="G77" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="I77" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="I77" s="2">
+      <c r="J77" s="2">
         <v>7</v>
       </c>
-      <c r="J77" s="2">
+      <c r="K77" s="2">
         <v>6</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="L77" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L77" s="2" t="s">
+      <c r="M77" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7">
         <v>1000130</v>
       </c>
@@ -4809,25 +5050,28 @@
         <v>416</v>
       </c>
       <c r="G78" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H78" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="I78" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="I78" s="2">
+      <c r="J78" s="2">
         <v>8</v>
       </c>
-      <c r="J78" s="2">
+      <c r="K78" s="2">
         <v>7</v>
       </c>
-      <c r="K78" s="2" t="s">
+      <c r="L78" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L78" s="2" t="s">
+      <c r="M78" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7">
         <v>1000008</v>
       </c>
@@ -4847,25 +5091,28 @@
         <v>417</v>
       </c>
       <c r="G79" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H79" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I79" s="4">
-        <v>1</v>
       </c>
       <c r="J79" s="4">
         <v>1</v>
       </c>
-      <c r="K79" s="4" t="s">
+      <c r="K79" s="4">
+        <v>1</v>
+      </c>
+      <c r="L79" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="L79" s="12" t="s">
+      <c r="M79" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="O79" s="4" t="s">
+      <c r="P79" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7">
         <v>1000075</v>
       </c>
@@ -4885,22 +5132,25 @@
         <v>417</v>
       </c>
       <c r="G80" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H80" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I80" s="2">
-        <v>1</v>
       </c>
       <c r="J80" s="2">
         <v>1</v>
       </c>
-      <c r="K80" s="2" t="s">
+      <c r="K80" s="2">
+        <v>1</v>
+      </c>
+      <c r="L80" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="M80" s="2" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7">
         <v>1000076</v>
       </c>
@@ -4920,22 +5170,25 @@
         <v>417</v>
       </c>
       <c r="G81" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H81" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I81" s="2">
+      <c r="J81" s="2">
         <v>1</v>
       </c>
-      <c r="J81" s="2">
-        <v>2</v>
-      </c>
-      <c r="K81" s="2" t="s">
+      <c r="K81" s="2">
+        <v>2</v>
+      </c>
+      <c r="L81" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L81" s="2" t="s">
+      <c r="M81" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7">
         <v>1000032</v>
       </c>
@@ -4955,21 +5208,24 @@
         <v>417</v>
       </c>
       <c r="G82" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H82" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I82" s="4">
+      <c r="J82" s="4">
         <v>1</v>
       </c>
-      <c r="J82" s="4"/>
-      <c r="K82" s="4" t="s">
+      <c r="K82" s="4"/>
+      <c r="L82" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L82" s="12" t="s">
+      <c r="M82" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="O82" s="4"/>
-    </row>
-    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P82" s="4"/>
+    </row>
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7">
         <v>1000033</v>
       </c>
@@ -4989,21 +5245,24 @@
         <v>417</v>
       </c>
       <c r="G83" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H83" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I83" s="4">
+      <c r="J83" s="4">
         <v>1</v>
       </c>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3" t="s">
+      <c r="K83" s="3"/>
+      <c r="L83" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L83" s="12" t="s">
+      <c r="M83" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="O83" s="3"/>
-    </row>
-    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P83" s="3"/>
+    </row>
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7">
         <v>1000051</v>
       </c>
@@ -5023,21 +5282,24 @@
         <v>417</v>
       </c>
       <c r="G84" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H84" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I84" s="4">
+      <c r="J84" s="4">
         <v>1</v>
       </c>
-      <c r="J84" s="4"/>
-      <c r="K84" s="4" t="s">
+      <c r="K84" s="4"/>
+      <c r="L84" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L84" s="12" t="s">
+      <c r="M84" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="O84" s="3"/>
-    </row>
-    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P84" s="3"/>
+    </row>
+    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7">
         <v>1000009</v>
       </c>
@@ -5057,23 +5319,26 @@
         <v>417</v>
       </c>
       <c r="G85" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H85" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I85" s="4">
-        <v>2</v>
-      </c>
       <c r="J85" s="4">
+        <v>2</v>
+      </c>
+      <c r="K85" s="4">
         <v>1</v>
       </c>
-      <c r="K85" s="4" t="s">
+      <c r="L85" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="L85" s="12" t="s">
+      <c r="M85" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="O85" s="3"/>
-    </row>
-    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P85" s="3"/>
+    </row>
+    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7">
         <v>1000015</v>
       </c>
@@ -5093,23 +5358,26 @@
         <v>417</v>
       </c>
       <c r="G86" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H86" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I86" s="4">
-        <v>2</v>
-      </c>
       <c r="J86" s="4">
         <v>2</v>
       </c>
-      <c r="K86" s="4" t="s">
+      <c r="K86" s="4">
+        <v>2</v>
+      </c>
+      <c r="L86" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="L86" s="12" t="s">
+      <c r="M86" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="O86" s="3"/>
-    </row>
-    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P86" s="3"/>
+    </row>
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7">
         <v>1000049</v>
       </c>
@@ -5129,23 +5397,26 @@
         <v>417</v>
       </c>
       <c r="G87" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H87" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I87" s="4">
-        <v>2</v>
-      </c>
       <c r="J87" s="4">
         <v>2</v>
       </c>
-      <c r="K87" s="4" t="s">
+      <c r="K87" s="4">
+        <v>2</v>
+      </c>
+      <c r="L87" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="L87" s="12" t="s">
+      <c r="M87" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="O87" s="3"/>
-    </row>
-    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P87" s="3"/>
+    </row>
+    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7">
         <v>1000078</v>
       </c>
@@ -5165,22 +5436,25 @@
         <v>417</v>
       </c>
       <c r="G88" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H88" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I88" s="2">
-        <v>2</v>
-      </c>
       <c r="J88" s="2">
         <v>2</v>
       </c>
-      <c r="K88" s="2" t="s">
+      <c r="K88" s="2">
+        <v>2</v>
+      </c>
+      <c r="L88" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L88" s="2" t="s">
+      <c r="M88" s="2" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7">
         <v>1000035</v>
       </c>
@@ -5200,21 +5474,24 @@
         <v>417</v>
       </c>
       <c r="G89" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H89" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I89" s="4">
-        <v>2</v>
-      </c>
-      <c r="J89" s="3"/>
-      <c r="K89" s="3" t="s">
+      <c r="J89" s="4">
+        <v>2</v>
+      </c>
+      <c r="K89" s="3"/>
+      <c r="L89" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="L89" s="12" t="s">
+      <c r="M89" s="12" t="s">
         <v>490</v>
       </c>
-      <c r="O89" s="3"/>
-    </row>
-    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P89" s="3"/>
+    </row>
+    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7">
         <v>1000080</v>
       </c>
@@ -5234,19 +5511,22 @@
         <v>417</v>
       </c>
       <c r="G90" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H90" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I90" s="2">
-        <v>2</v>
-      </c>
-      <c r="K90" s="2" t="s">
+      <c r="J90" s="2">
+        <v>2</v>
+      </c>
+      <c r="L90" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L90" s="2" t="s">
+      <c r="M90" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7">
         <v>1000079</v>
       </c>
@@ -5266,19 +5546,22 @@
         <v>417</v>
       </c>
       <c r="G91" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H91" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I91" s="2">
-        <v>2</v>
-      </c>
-      <c r="K91" s="2" t="s">
+      <c r="J91" s="2">
+        <v>2</v>
+      </c>
+      <c r="L91" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L91" s="2" t="s">
+      <c r="M91" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7">
         <v>1000081</v>
       </c>
@@ -5298,19 +5581,22 @@
         <v>417</v>
       </c>
       <c r="G92" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H92" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I92" s="2">
-        <v>2</v>
-      </c>
-      <c r="K92" s="2" t="s">
+      <c r="J92" s="2">
+        <v>2</v>
+      </c>
+      <c r="L92" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L92" s="2" t="s">
+      <c r="M92" s="2" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7">
         <v>1000083</v>
       </c>
@@ -5330,19 +5616,22 @@
         <v>417</v>
       </c>
       <c r="G93" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H93" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I93" s="2">
-        <v>2</v>
-      </c>
-      <c r="K93" s="2" t="s">
+      <c r="J93" s="2">
+        <v>2</v>
+      </c>
+      <c r="L93" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L93" s="2" t="s">
+      <c r="M93" s="2" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="7">
         <v>1000050</v>
       </c>
@@ -5362,23 +5651,26 @@
         <v>417</v>
       </c>
       <c r="G94" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H94" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I94" s="4">
-        <v>3</v>
       </c>
       <c r="J94" s="4">
         <v>3</v>
       </c>
-      <c r="K94" s="4" t="s">
+      <c r="K94" s="4">
+        <v>3</v>
+      </c>
+      <c r="L94" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="L94" s="12" t="s">
+      <c r="M94" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="O94" s="3"/>
-    </row>
-    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P94" s="3"/>
+    </row>
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7">
         <v>1000085</v>
       </c>
@@ -5398,22 +5690,25 @@
         <v>417</v>
       </c>
       <c r="G95" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H95" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I95" s="2">
-        <v>3</v>
       </c>
       <c r="J95" s="2">
         <v>3</v>
       </c>
-      <c r="K95" s="2" t="s">
+      <c r="K95" s="2">
+        <v>3</v>
+      </c>
+      <c r="L95" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L95" s="2" t="s">
+      <c r="M95" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7">
         <v>1000086</v>
       </c>
@@ -5433,22 +5728,25 @@
         <v>417</v>
       </c>
       <c r="G96" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H96" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I96" s="2">
+      <c r="J96" s="2">
         <v>3</v>
       </c>
-      <c r="J96" s="2">
+      <c r="K96" s="2">
         <v>4</v>
       </c>
-      <c r="K96" s="2" t="s">
+      <c r="L96" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L96" s="2" t="s">
+      <c r="M96" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
         <v>1000036</v>
       </c>
@@ -5468,21 +5766,24 @@
         <v>417</v>
       </c>
       <c r="G97" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H97" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I97" s="4">
+      <c r="J97" s="4">
         <v>3</v>
       </c>
-      <c r="J97" s="3"/>
-      <c r="K97" s="3" t="s">
+      <c r="K97" s="3"/>
+      <c r="L97" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="L97" s="12" t="s">
+      <c r="M97" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="O97" s="3"/>
-    </row>
-    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P97" s="3"/>
+    </row>
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7">
         <v>1000077</v>
       </c>
@@ -5502,19 +5803,22 @@
         <v>417</v>
       </c>
       <c r="G98" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H98" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I98" s="2">
+      <c r="J98" s="2">
         <v>3</v>
       </c>
-      <c r="K98" s="2" t="s">
+      <c r="L98" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L98" s="2" t="s">
+      <c r="M98" s="2" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>1000034</v>
       </c>
@@ -5534,21 +5838,24 @@
         <v>417</v>
       </c>
       <c r="G99" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H99" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I99" s="4">
+      <c r="J99" s="4">
         <v>3</v>
       </c>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3" t="s">
+      <c r="K99" s="3"/>
+      <c r="L99" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L99" s="12" t="s">
+      <c r="M99" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="O99" s="3"/>
-    </row>
-    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P99" s="3"/>
+    </row>
+    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7">
         <v>1000088</v>
       </c>
@@ -5568,19 +5875,22 @@
         <v>417</v>
       </c>
       <c r="G100" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H100" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I100" s="2">
+      <c r="J100" s="2">
         <v>3</v>
       </c>
-      <c r="K100" s="2" t="s">
+      <c r="L100" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L100" s="2" t="s">
+      <c r="M100" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7">
         <v>1000089</v>
       </c>
@@ -5600,19 +5910,22 @@
         <v>417</v>
       </c>
       <c r="G101" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H101" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I101" s="2">
+      <c r="J101" s="2">
         <v>3</v>
       </c>
-      <c r="K101" s="2" t="s">
+      <c r="L101" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L101" s="2" t="s">
+      <c r="M101" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7">
         <v>1000092</v>
       </c>
@@ -5632,19 +5945,22 @@
         <v>417</v>
       </c>
       <c r="G102" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H102" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I102" s="2">
+      <c r="J102" s="2">
         <v>3</v>
       </c>
-      <c r="K102" s="2" t="s">
+      <c r="L102" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L102" s="2" t="s">
+      <c r="M102" s="2" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7">
         <v>1000022</v>
       </c>
@@ -5664,23 +5980,26 @@
         <v>417</v>
       </c>
       <c r="G103" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H103" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I103" s="4">
+      <c r="J103" s="4">
         <v>4</v>
       </c>
-      <c r="J103" s="4">
-        <v>2</v>
-      </c>
-      <c r="K103" s="4" t="s">
+      <c r="K103" s="4">
+        <v>2</v>
+      </c>
+      <c r="L103" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="L103" s="12" t="s">
+      <c r="M103" s="12" t="s">
         <v>496</v>
       </c>
-      <c r="O103" s="3"/>
-    </row>
-    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P103" s="3"/>
+    </row>
+    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7">
         <v>1000090</v>
       </c>
@@ -5700,19 +6019,22 @@
         <v>417</v>
       </c>
       <c r="G104" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H104" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I104" s="2">
+      <c r="J104" s="2">
         <v>4</v>
       </c>
-      <c r="K104" s="2" t="s">
+      <c r="L104" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L104" s="2" t="s">
+      <c r="M104" s="2" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7">
         <v>1000091</v>
       </c>
@@ -5732,19 +6054,22 @@
         <v>417</v>
       </c>
       <c r="G105" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H105" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I105" s="2">
+      <c r="J105" s="2">
         <v>4</v>
       </c>
-      <c r="K105" s="2" t="s">
+      <c r="L105" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L105" s="2" t="s">
+      <c r="M105" s="2" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7">
         <v>1000026</v>
       </c>
@@ -5764,26 +6089,29 @@
         <v>417</v>
       </c>
       <c r="G106" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H106" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H106" s="2" t="s">
+      <c r="I106" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="I106" s="4">
-        <v>5</v>
       </c>
       <c r="J106" s="4">
         <v>5</v>
       </c>
-      <c r="K106" s="4" t="s">
+      <c r="K106" s="4">
+        <v>5</v>
+      </c>
+      <c r="L106" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="L106" s="12" t="s">
+      <c r="M106" s="12" t="s">
         <v>499</v>
       </c>
-      <c r="O106" s="3"/>
-    </row>
-    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P106" s="3"/>
+    </row>
+    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7">
         <v>1000082</v>
       </c>
@@ -5803,19 +6131,22 @@
         <v>417</v>
       </c>
       <c r="G107" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H107" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I107" s="2">
+      <c r="J107" s="2">
         <v>5</v>
       </c>
-      <c r="K107" s="2" t="s">
+      <c r="L107" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L107" s="2" t="s">
+      <c r="M107" s="2" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7">
         <v>1000094</v>
       </c>
@@ -5835,22 +6166,25 @@
         <v>417</v>
       </c>
       <c r="G108" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H108" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I108" s="2">
+      <c r="J108" s="2">
         <v>6</v>
       </c>
-      <c r="J108" s="2">
+      <c r="K108" s="2">
         <v>7</v>
       </c>
-      <c r="K108" s="2" t="s">
+      <c r="L108" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L108" s="2" t="s">
+      <c r="M108" s="2" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7">
         <v>1000093</v>
       </c>
@@ -5870,19 +6204,22 @@
         <v>417</v>
       </c>
       <c r="G109" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H109" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I109" s="2">
+      <c r="J109" s="2">
         <v>6</v>
       </c>
-      <c r="K109" s="2" t="s">
+      <c r="L109" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L109" s="2" t="s">
+      <c r="M109" s="2" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7">
         <v>1000087</v>
       </c>
@@ -5902,22 +6239,25 @@
         <v>417</v>
       </c>
       <c r="G110" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H110" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I110" s="2">
-        <v>7</v>
       </c>
       <c r="J110" s="2">
         <v>7</v>
       </c>
-      <c r="K110" s="2" t="s">
+      <c r="K110" s="2">
+        <v>7</v>
+      </c>
+      <c r="L110" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L110" s="2" t="s">
+      <c r="M110" s="2" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7">
         <v>1000084</v>
       </c>
@@ -5937,22 +6277,25 @@
         <v>417</v>
       </c>
       <c r="G111" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H111" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I111" s="2">
+      <c r="J111" s="2">
         <v>8</v>
       </c>
-      <c r="J111" s="2">
+      <c r="K111" s="2">
         <v>7</v>
       </c>
-      <c r="K111" s="2" t="s">
+      <c r="L111" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L111" s="2" t="s">
+      <c r="M111" s="2" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7">
         <v>1000095</v>
       </c>
@@ -5972,25 +6315,28 @@
         <v>418</v>
       </c>
       <c r="G112" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H112" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H112" s="2" t="s">
+      <c r="I112" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="I112" s="2">
-        <v>1</v>
       </c>
       <c r="J112" s="2">
         <v>1</v>
       </c>
-      <c r="K112" s="2" t="s">
+      <c r="K112" s="2">
+        <v>1</v>
+      </c>
+      <c r="L112" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L112" s="2" t="s">
+      <c r="M112" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7">
         <v>1000096</v>
       </c>
@@ -6010,22 +6356,25 @@
         <v>418</v>
       </c>
       <c r="G113" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H113" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I113" s="2">
-        <v>1</v>
       </c>
       <c r="J113" s="2">
         <v>1</v>
       </c>
-      <c r="K113" s="2" t="s">
+      <c r="K113" s="2">
+        <v>1</v>
+      </c>
+      <c r="L113" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L113" s="2" t="s">
+      <c r="M113" s="2" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7">
         <v>1000097</v>
       </c>
@@ -6045,22 +6394,25 @@
         <v>418</v>
       </c>
       <c r="G114" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H114" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I114" s="2">
-        <v>1</v>
       </c>
       <c r="J114" s="2">
         <v>1</v>
       </c>
-      <c r="K114" s="2" t="s">
+      <c r="K114" s="2">
+        <v>1</v>
+      </c>
+      <c r="L114" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L114" s="2" t="s">
+      <c r="M114" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>1000101</v>
       </c>
@@ -6080,19 +6432,22 @@
         <v>418</v>
       </c>
       <c r="G115" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H115" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I115" s="2">
+      <c r="J115" s="2">
         <v>1</v>
       </c>
-      <c r="K115" s="2" t="s">
+      <c r="L115" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L115" s="2" t="s">
+      <c r="M115" s="2" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7">
         <v>1000102</v>
       </c>
@@ -6112,19 +6467,22 @@
         <v>418</v>
       </c>
       <c r="G116" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H116" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I116" s="2">
+      <c r="J116" s="2">
         <v>1</v>
       </c>
-      <c r="K116" s="2" t="s">
+      <c r="L116" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L116" s="2" t="s">
+      <c r="M116" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
         <v>1000037</v>
       </c>
@@ -6144,21 +6502,24 @@
         <v>418</v>
       </c>
       <c r="G117" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H117" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I117" s="4">
+      <c r="J117" s="4">
         <v>1</v>
       </c>
-      <c r="J117" s="3"/>
-      <c r="K117" s="3" t="s">
+      <c r="K117" s="3"/>
+      <c r="L117" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L117" s="12" t="s">
+      <c r="M117" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="O117" s="3"/>
-    </row>
-    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P117" s="3"/>
+    </row>
+    <row r="118" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7">
         <v>1000099</v>
       </c>
@@ -6178,19 +6539,22 @@
         <v>418</v>
       </c>
       <c r="G118" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H118" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I118" s="2">
+      <c r="J118" s="2">
         <v>1</v>
       </c>
-      <c r="K118" s="2" t="s">
+      <c r="L118" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L118" s="2" t="s">
+      <c r="M118" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7">
         <v>1000100</v>
       </c>
@@ -6210,19 +6574,22 @@
         <v>418</v>
       </c>
       <c r="G119" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H119" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I119" s="2">
+      <c r="J119" s="2">
         <v>1</v>
       </c>
-      <c r="K119" s="2" t="s">
+      <c r="L119" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L119" s="2" t="s">
+      <c r="M119" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
         <v>1000103</v>
       </c>
@@ -6242,25 +6609,28 @@
         <v>418</v>
       </c>
       <c r="G120" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H120" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H120" s="2" t="s">
+      <c r="I120" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="I120" s="2">
-        <v>2</v>
-      </c>
       <c r="J120" s="2">
         <v>2</v>
       </c>
-      <c r="K120" s="2" t="s">
+      <c r="K120" s="2">
+        <v>2</v>
+      </c>
+      <c r="L120" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L120" s="2" t="s">
+      <c r="M120" s="2" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7">
         <v>1000105</v>
       </c>
@@ -6280,22 +6650,25 @@
         <v>418</v>
       </c>
       <c r="G121" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H121" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I121" s="2">
-        <v>2</v>
-      </c>
       <c r="J121" s="2">
+        <v>2</v>
+      </c>
+      <c r="K121" s="2">
         <v>0</v>
       </c>
-      <c r="K121" s="2" t="s">
+      <c r="L121" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L121" s="2" t="s">
+      <c r="M121" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7">
         <v>1000106</v>
       </c>
@@ -6315,25 +6688,28 @@
         <v>418</v>
       </c>
       <c r="G122" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H122" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H122" s="2" t="s">
+      <c r="I122" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="I122" s="2">
-        <v>2</v>
-      </c>
       <c r="J122" s="2">
         <v>2</v>
       </c>
-      <c r="K122" s="2" t="s">
+      <c r="K122" s="2">
+        <v>2</v>
+      </c>
+      <c r="L122" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L122" s="2" t="s">
+      <c r="M122" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7">
         <v>1000038</v>
       </c>
@@ -6353,21 +6729,24 @@
         <v>418</v>
       </c>
       <c r="G123" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H123" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I123" s="4">
-        <v>2</v>
-      </c>
-      <c r="J123" s="4"/>
-      <c r="K123" s="4" t="s">
+      <c r="J123" s="4">
+        <v>2</v>
+      </c>
+      <c r="K123" s="4"/>
+      <c r="L123" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L123" s="12" t="s">
+      <c r="M123" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="O123" s="3"/>
-    </row>
-    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P123" s="3"/>
+    </row>
+    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7">
         <v>1000107</v>
       </c>
@@ -6387,19 +6766,22 @@
         <v>418</v>
       </c>
       <c r="G124" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H124" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I124" s="2">
-        <v>2</v>
-      </c>
-      <c r="K124" s="2" t="s">
+      <c r="J124" s="2">
+        <v>2</v>
+      </c>
+      <c r="L124" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L124" s="2" t="s">
+      <c r="M124" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7">
         <v>1000108</v>
       </c>
@@ -6419,19 +6801,22 @@
         <v>418</v>
       </c>
       <c r="G125" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H125" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I125" s="2">
-        <v>2</v>
-      </c>
-      <c r="K125" s="2" t="s">
+      <c r="J125" s="2">
+        <v>2</v>
+      </c>
+      <c r="L125" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L125" s="2" t="s">
+      <c r="M125" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7">
         <v>1000109</v>
       </c>
@@ -6451,19 +6836,22 @@
         <v>418</v>
       </c>
       <c r="G126" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H126" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I126" s="2">
-        <v>2</v>
-      </c>
-      <c r="K126" s="2" t="s">
+      <c r="J126" s="2">
+        <v>2</v>
+      </c>
+      <c r="L126" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L126" s="2" t="s">
+      <c r="M126" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7">
         <v>1000112</v>
       </c>
@@ -6483,25 +6871,28 @@
         <v>418</v>
       </c>
       <c r="G127" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H127" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H127" s="2" t="s">
+      <c r="I127" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="I127" s="2">
-        <v>3</v>
       </c>
       <c r="J127" s="2">
         <v>3</v>
       </c>
-      <c r="K127" s="2" t="s">
+      <c r="K127" s="2">
+        <v>3</v>
+      </c>
+      <c r="L127" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L127" s="2" t="s">
+      <c r="M127" s="2" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7">
         <v>1000137</v>
       </c>
@@ -6518,22 +6909,25 @@
         <v>418</v>
       </c>
       <c r="G128" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H128" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I128" s="2">
-        <v>3</v>
       </c>
       <c r="J128" s="2">
         <v>3</v>
       </c>
-      <c r="K128" s="2" t="s">
+      <c r="K128" s="2">
+        <v>3</v>
+      </c>
+      <c r="L128" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L128" s="2" t="s">
+      <c r="M128" s="2" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7">
         <v>1000116</v>
       </c>
@@ -6553,19 +6947,22 @@
         <v>418</v>
       </c>
       <c r="G129" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H129" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="I129" s="2">
+      <c r="J129" s="2">
         <v>3</v>
       </c>
-      <c r="K129" s="2" t="s">
+      <c r="L129" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="L129" s="2" t="s">
+      <c r="M129" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7">
         <v>1000041</v>
       </c>
@@ -6585,21 +6982,24 @@
         <v>418</v>
       </c>
       <c r="G130" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H130" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I130" s="4">
+      <c r="J130" s="4">
         <v>3</v>
       </c>
-      <c r="J130" s="4"/>
-      <c r="K130" s="4" t="s">
+      <c r="K130" s="4"/>
+      <c r="L130" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L130" s="12" t="s">
+      <c r="M130" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="O130" s="3"/>
-    </row>
-    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+      <c r="P130" s="3"/>
+    </row>
+    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7">
         <v>1000098</v>
       </c>
@@ -6619,25 +7019,28 @@
         <v>418</v>
       </c>
       <c r="G131" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H131" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H131" s="2" t="s">
+      <c r="I131" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="I131" s="2">
+      <c r="J131" s="2">
         <v>4</v>
       </c>
-      <c r="J131" s="2">
+      <c r="K131" s="2">
         <v>3</v>
       </c>
-      <c r="K131" s="2" t="s">
+      <c r="L131" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="L131" s="2" t="s">
+      <c r="M131" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7">
         <v>1000138</v>
       </c>
@@ -6654,22 +7057,25 @@
         <v>418</v>
       </c>
       <c r="G132" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H132" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I132" s="2">
-        <v>4</v>
       </c>
       <c r="J132" s="2">
         <v>4</v>
       </c>
-      <c r="K132" s="2" t="s">
+      <c r="K132" s="2">
+        <v>4</v>
+      </c>
+      <c r="L132" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="L132" s="2" t="s">
+      <c r="M132" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7">
         <v>1000115</v>
       </c>
@@ -6689,19 +7095,22 @@
         <v>418</v>
       </c>
       <c r="G133" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H133" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I133" s="2">
+      <c r="J133" s="2">
         <v>4</v>
       </c>
-      <c r="K133" s="2" t="s">
+      <c r="L133" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L133" s="2" t="s">
+      <c r="M133" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="134" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7">
         <v>1000113</v>
       </c>
@@ -6721,22 +7130,25 @@
         <v>418</v>
       </c>
       <c r="G134" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H134" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="I134" s="2">
-        <v>5</v>
       </c>
       <c r="J134" s="2">
         <v>5</v>
       </c>
-      <c r="K134" s="2" t="s">
+      <c r="K134" s="2">
+        <v>5</v>
+      </c>
+      <c r="L134" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L134" s="2" t="s">
+      <c r="M134" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7">
         <v>1000111</v>
       </c>
@@ -6756,19 +7168,22 @@
         <v>418</v>
       </c>
       <c r="G135" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H135" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I135" s="2">
+      <c r="J135" s="2">
         <v>5</v>
       </c>
-      <c r="K135" s="2" t="s">
+      <c r="L135" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="L135" s="2" t="s">
+      <c r="M135" s="2" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7">
         <v>1000104</v>
       </c>
@@ -6788,22 +7203,25 @@
         <v>418</v>
       </c>
       <c r="G136" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H136" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I136" s="2">
+      <c r="J136" s="2">
         <v>6</v>
       </c>
-      <c r="J136" s="2">
-        <v>2</v>
-      </c>
-      <c r="K136" s="2" t="s">
+      <c r="K136" s="2">
+        <v>2</v>
+      </c>
+      <c r="L136" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L136" s="2" t="s">
+      <c r="M136" s="2" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7">
         <v>1000117</v>
       </c>
@@ -6823,22 +7241,25 @@
         <v>418</v>
       </c>
       <c r="G137" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H137" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I137" s="2">
+      <c r="J137" s="2">
         <v>6</v>
       </c>
-      <c r="J137" s="2">
+      <c r="K137" s="2">
         <v>4</v>
       </c>
-      <c r="K137" s="2" t="s">
+      <c r="L137" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L137" s="2" t="s">
+      <c r="M137" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7">
         <v>1000110</v>
       </c>
@@ -6858,25 +7279,28 @@
         <v>418</v>
       </c>
       <c r="G138" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H138" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H138" s="2" t="s">
+      <c r="I138" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="I138" s="2">
+      <c r="J138" s="2">
         <v>7</v>
       </c>
-      <c r="J138" s="2">
+      <c r="K138" s="2">
         <v>5</v>
       </c>
-      <c r="K138" s="2" t="s">
+      <c r="L138" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L138" s="2" t="s">
+      <c r="M138" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7">
         <v>1000114</v>
       </c>
@@ -6896,42 +7320,45 @@
         <v>418</v>
       </c>
       <c r="G139" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="H139" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="I139" s="2">
+      <c r="J139" s="2">
         <v>8</v>
       </c>
-      <c r="J139" s="2">
+      <c r="K139" s="2">
         <v>5</v>
       </c>
-      <c r="K139" s="2" t="s">
+      <c r="L139" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="L139" s="2" t="s">
+      <c r="M139" s="2" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="7">
         <v>1000139</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="7">
         <v>1000140</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="7">
         <v>1000141</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="7">
         <v>1000142</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="7">
         <v>1000143</v>
       </c>
@@ -11217,7 +11644,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1000" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:P1000" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="4">
       <filters blank="1">
         <filter val="Aether"/>
@@ -11228,13 +11655,13 @@
         <filter val="blue"/>
       </filters>
     </filterColumn>
-    <sortState ref="A6:O1000">
+    <sortState ref="A6:P1000">
       <sortCondition ref="F1:F1000"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A2:O128">
-    <sortCondition ref="I2:I1000"/>
-    <sortCondition ref="G2:G1000"/>
+  <sortState ref="A2:P128">
+    <sortCondition ref="J2:J1000"/>
+    <sortCondition ref="H2:H1000"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11246,7 +11673,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11511,19 +11938,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A2,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A2,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>4</v>
       </c>
       <c r="C2" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A2,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A2,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>4</v>
       </c>
       <c r="D2" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A2,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A2,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>4</v>
       </c>
       <c r="E2" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A2,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A2,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>4</v>
       </c>
       <c r="F2" s="5">
@@ -11535,19 +11962,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A3,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A3,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>4</v>
       </c>
       <c r="C3" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A3,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A3,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>4</v>
       </c>
       <c r="D3" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A3,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A3,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>4</v>
       </c>
       <c r="E3" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A3,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A3,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>4</v>
       </c>
       <c r="F3" s="5">
@@ -11559,19 +11986,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A4,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A4,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>3</v>
       </c>
       <c r="C4" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A4,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A4,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>3</v>
       </c>
       <c r="D4" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A4,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A4,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>3</v>
       </c>
       <c r="E4" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A4,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A4,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>3</v>
       </c>
       <c r="F4" s="5">
@@ -11583,19 +12010,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A5,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A5,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>3</v>
       </c>
       <c r="C5" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A5,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A5,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>3</v>
       </c>
       <c r="D5" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A5,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A5,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>3</v>
       </c>
       <c r="E5" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A5,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A5,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>3</v>
       </c>
       <c r="F5" s="5">
@@ -11607,19 +12034,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A6,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A6,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A6,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A6,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>2</v>
       </c>
       <c r="D6" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A6,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A6,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>2</v>
       </c>
       <c r="E6" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A6,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A6,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>2</v>
       </c>
       <c r="F6" s="5">
@@ -11631,19 +12058,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A7,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A7,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>2</v>
       </c>
       <c r="C7" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A7,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A7,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>2</v>
       </c>
       <c r="D7" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A7,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A7,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>2</v>
       </c>
       <c r="E7" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A7,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A7,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>2</v>
       </c>
       <c r="F7" s="5">
@@ -11655,19 +12082,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A8,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A8,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>1</v>
       </c>
       <c r="C8" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A8,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A8,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>1</v>
       </c>
       <c r="D8" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A8,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A8,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A8,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A8,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>1</v>
       </c>
       <c r="F8" s="5">
@@ -11679,19 +12106,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A9,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A9,Card!$F:$F,"="&amp;B$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A9,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A9,Card!$F:$F,"="&amp;C$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>1</v>
       </c>
       <c r="D9" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A9,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A9,Card!$F:$F,"="&amp;D$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>1</v>
       </c>
       <c r="E9" s="5">
-        <f>COUNTIFS(Card!$I:$I,"="&amp;$A9,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
+        <f>COUNTIFS(Card!$J:$J,"="&amp;$A9,Card!$F:$F,"="&amp;E$1,Card!$E:$E,"="&amp;$H$1)</f>
         <v>1</v>
       </c>
       <c r="F9" s="5">
@@ -11733,8 +12160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4DD316-5D31-42C7-BA9E-706018F97981}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11766,7 +12193,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -11782,7 +12209,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -11830,7 +12257,7 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -11846,7 +12273,7 @@
         <v>2</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>